<commit_message>
matrici giornalieri con turni da 7 ore database aggiornato con il turno di settembre 2016
</commit_message>
<xml_diff>
--- a/DATABASE/matriciOSA.xlsx
+++ b/DATABASE/matriciOSA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="975" windowWidth="19320" windowHeight="11790"/>
@@ -13,7 +13,7 @@
     <sheet name="xl_DCF_History" sheetId="4" state="veryHidden" r:id="rId4"/>
     <sheet name="Classified as UnClassified" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -360,1240 +360,9 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="123">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1607,7 +376,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1894,12 +663,12 @@
   <dimension ref="A1:M76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="M59" sqref="M59:M76"/>
+      <selection activeCell="C71" sqref="C71:I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -4782,25 +3551,25 @@
         <v>35</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E71" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F71" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G71" s="17" t="s">
         <v>9</v>
       </c>
       <c r="H71" s="16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I71" s="16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>50</v>
@@ -4823,25 +3592,25 @@
         <v>36</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D72" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E72" s="19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F72" s="17" t="s">
         <v>9</v>
       </c>
       <c r="G72" s="19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H72" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I72" s="19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>50</v>
@@ -4864,25 +3633,25 @@
         <v>37</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D73" s="19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E73" s="17" t="s">
         <v>9</v>
       </c>
       <c r="F73" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G73" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H73" s="19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I73" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>50</v>
@@ -4905,25 +3674,25 @@
         <v>38</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D74" s="17" t="s">
         <v>9</v>
       </c>
       <c r="E74" s="19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F74" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G74" s="19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H74" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I74" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>50</v>

</xml_diff>